<commit_message>
add submission set genes statistics back
</commit_message>
<xml_diff>
--- a/Pubmed/Nipah/ReferenceSummary_Dec11.xlsx
+++ b/Pubmed/Nipah/ReferenceSummary_Dec11.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/Library/CloudStorage/Dropbox/Shared/___SystematicReviewsAI/Nipah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C14487-5D48-434C-9852-ED0046263B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F532CA-CE5D-B546-80D5-C06E57924244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="760" windowWidth="34560" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="760" windowWidth="34560" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="481">
   <si>
     <t>Title</t>
   </si>
@@ -1522,6 +1522,24 @@
   </si>
   <si>
     <t>CloneMethod</t>
+  </si>
+  <si>
+    <t>Determination of the henipavirus phosphoprotein gene mRNA editing frequencies and detection of the C, V and W proteins of Nipah virus in virus-infected cells.</t>
+  </si>
+  <si>
+    <t>Lo MK; Harcourt BH; Mungall BA; Tamin A; Peeples ME; Bellini WJ; Rota PA</t>
+  </si>
+  <si>
+    <t>Both human and GPT said 'Unlikely', but it's one of the Genbank Submission set.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>infected cell cultures​</t>
+  </si>
+  <si>
+    <t>virus-infected cell lysates</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1582,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1579,6 +1597,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1624,7 +1648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1645,6 +1669,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1947,11 +1972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C70" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C77" sqref="A76:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2210,7 +2234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2426,7 +2450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -2805,7 +2829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -2953,7 +2977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -3024,7 +3048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -3095,7 +3119,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3238,7 +3262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3306,7 +3330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -3377,7 +3401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3522,7 +3546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
@@ -3572,7 +3596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
@@ -3693,7 +3717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
@@ -3752,7 +3776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>73</v>
       </c>
@@ -3802,7 +3826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
@@ -3873,7 +3897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -3938,7 +3962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4006,7 +4030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
@@ -4074,7 +4098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>84</v>
       </c>
@@ -4219,7 +4243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>89</v>
       </c>
@@ -4367,7 +4391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>94</v>
       </c>
@@ -4438,7 +4462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>97</v>
       </c>
@@ -4488,7 +4512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>100</v>
       </c>
@@ -4633,7 +4657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>105</v>
       </c>
@@ -4846,7 +4870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>113</v>
       </c>
@@ -4917,7 +4941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>115</v>
       </c>
@@ -4988,7 +5012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>117</v>
       </c>
@@ -5038,7 +5062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>120</v>
       </c>
@@ -5085,7 +5109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>123</v>
       </c>
@@ -5156,7 +5180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>125</v>
       </c>
@@ -5277,7 +5301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>129</v>
       </c>
@@ -5324,7 +5348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>132</v>
       </c>
@@ -5395,7 +5419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>134</v>
       </c>
@@ -5442,7 +5466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>136</v>
       </c>
@@ -5513,7 +5537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>139</v>
       </c>
@@ -5652,7 +5676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>143</v>
       </c>
@@ -5723,7 +5747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>145</v>
       </c>
@@ -5794,7 +5818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>147</v>
       </c>
@@ -5995,7 +6019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>155</v>
       </c>
@@ -6066,7 +6090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>158</v>
       </c>
@@ -6122,7 +6146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>160</v>
       </c>
@@ -6193,7 +6217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>163</v>
       </c>
@@ -6264,7 +6288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>165</v>
       </c>
@@ -6317,7 +6341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>168</v>
       </c>
@@ -6565,7 +6589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>177</v>
       </c>
@@ -6710,7 +6734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>418</v>
       </c>
@@ -6775,7 +6799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>420</v>
       </c>
@@ -6825,7 +6849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" ht="80" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>422</v>
       </c>
@@ -6893,7 +6917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>424</v>
       </c>
@@ -6955,7 +6979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="176" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" ht="176" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>426</v>
       </c>
@@ -7017,51 +7041,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="B76" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="C76">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="D76" t="s">
-        <v>471</v>
+        <v>162</v>
       </c>
       <c r="E76">
-        <v>32288829</v>
+        <v>19141449</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M76" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="Q76" s="8" t="s">
+        <v>477</v>
       </c>
       <c r="R76" s="7" t="s">
         <v>9</v>
       </c>
       <c r="U76" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="Y76" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="Y76" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B77" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C77">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="D77" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E77">
-        <v>12722231</v>
+        <v>32288829</v>
       </c>
       <c r="R77" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="S77" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="T77" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="U77" s="3" t="s">
         <v>472</v>
       </c>
@@ -7069,19 +7123,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="78" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>468</v>
+      </c>
+      <c r="B78" t="s">
+        <v>469</v>
+      </c>
+      <c r="C78">
+        <v>2003</v>
+      </c>
+      <c r="D78" t="s">
+        <v>470</v>
+      </c>
+      <c r="E78">
+        <v>12722231</v>
+      </c>
+      <c r="R78" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="T78" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Y77" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="18">
-      <filters>
-        <filter val="No"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="21">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Y75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>